<commit_message>
[양선욱] SelectStatTable 수정 완료
[양선욱] SelectStatTable 수정 완료
</commit_message>
<xml_diff>
--- a/Assets/ExcelDatas/SelectStatData.xlsx
+++ b/Assets/ExcelDatas/SelectStatData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vcds1\Documents\GitHub\Project_Advence\Assets\ExcelDatas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7765BB-A2F3-4E0A-9C20-06A7BBCDFE60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD41628-4A32-4420-B701-12FE990DCBFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" firstSheet="1" activeTab="1" xr2:uid="{00B68857-C6E1-4D98-82FE-3C4F502D76E8}"/>
   </bookViews>
@@ -305,7 +305,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>ALL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -499,35 +499,39 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>모든 스킬의 피해량을 강화 합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 스킬의 공격속도를 강화 합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>이동속도를 강화 합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>방어력을 강화 합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>모든 스킬의 크리티컬 데미지를 강화 합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>지속적으로 체력을 회복합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>체력을 즉시 회복합니다</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SelectStatName 인자값 설명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>{0}: EnchantEffectValue1 * 100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이동속도를 {0}% 강화 합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 스킬의 공격속도를 {0}% 강화 합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 스킬의 피해량을 {0}% 강화 합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>방어력을 {0}% 강화 합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>모든 스킬의 크리티컬 데미지를 {0}% 강화 합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>체력을 즉시 {0}% 회복합니다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>초당 체력을 {0}% 회복합니다</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -816,7 +820,7 @@
         <name val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
-        <scheme val="none"/>
+        <scheme val="major"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -832,7 +836,7 @@
         <name val="맑은 고딕"/>
         <family val="3"/>
         <charset val="129"/>
-        <scheme val="major"/>
+        <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1178,8 +1182,8 @@
     <tableColumn id="3" xr3:uid="{879C8458-55D3-490C-B008-37FEB8ADB40B}" name="SelectStatRateValue" dataDxfId="4"/>
     <tableColumn id="5" xr3:uid="{C9F5527E-5E1B-4F02-AE48-4C86428FE4F7}" name="Description" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{33292A04-0117-400B-AAB3-C905E7D91CE1}" name="Icon" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{A3184252-0CAA-4A91-AED0-77A8B48C7CAF}" name="MaxCount" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{C6BA0C5D-D868-4187-8D0D-E128920DD621}" name="SelectStatName 인자값 설명" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{A3184252-0CAA-4A91-AED0-77A8B48C7CAF}" name="MaxCount" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{C6BA0C5D-D868-4187-8D0D-E128920DD621}" name="SelectStatName 인자값 설명" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1655,7 +1659,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.2" x14ac:dyDescent="0.4"/>
@@ -1746,7 +1750,7 @@
         <v>29</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.4">
@@ -1760,10 +1764,10 @@
         <v>6</v>
       </c>
       <c r="D4" s="2">
-        <v>0.5</v>
+        <v>0.05</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F4" s="20" t="s">
         <v>40</v>
@@ -1771,7 +1775,9 @@
       <c r="G4" s="20">
         <v>5</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
@@ -1784,10 +1790,10 @@
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F5" s="20" t="s">
         <v>41</v>
@@ -1795,7 +1801,9 @@
       <c r="G5" s="20">
         <v>5</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
@@ -1808,7 +1816,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>51</v>
@@ -1819,7 +1827,9 @@
       <c r="G6" s="20">
         <v>5</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
@@ -1832,10 +1842,10 @@
         <v>10</v>
       </c>
       <c r="D7" s="2">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="20" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="F7" s="20" t="s">
         <v>45</v>
@@ -1843,7 +1853,9 @@
       <c r="G7" s="20">
         <v>5</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
@@ -1859,7 +1871,7 @@
         <v>0.5</v>
       </c>
       <c r="E8" s="20" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F8" s="20" t="s">
         <v>46</v>
@@ -1867,7 +1879,9 @@
       <c r="G8" s="20">
         <v>5</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
@@ -1883,7 +1897,7 @@
         <v>1E-3</v>
       </c>
       <c r="E9" s="20" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="F9" s="20" t="s">
         <v>43</v>
@@ -1891,7 +1905,9 @@
       <c r="G9" s="20">
         <v>3</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
@@ -1907,7 +1923,7 @@
         <v>0.7</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="F10" s="20" t="s">
         <v>44</v>
@@ -1915,7 +1931,9 @@
       <c r="G10" s="20">
         <v>99</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="H11" s="2"/>

</xml_diff>